<commit_message>
SSDM-13256: Added Registration Date, Registrator, Modification Date and Modifier export support for data sets.
</commit_message>
<xml_diff>
--- a/server-application-server/sourceTest/java/ch/ethz/sis/openbis/generic/server/xls/export/resources/export-data-set-filtered-fields.xlsx
+++ b/server-application-server/sourceTest/java/ch/ethz/sis/openbis/generic/server/xls/export/resources/export-data-set-filtered-fields.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="28">
   <si>
     <t xml:space="preserve">DATASET</t>
   </si>
@@ -40,6 +40,12 @@
     <t xml:space="preserve">Attachment</t>
   </si>
   <si>
+    <t xml:space="preserve">Registration Date</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Registrator</t>
+  </si>
+  <si>
     <t xml:space="preserve">TEST_2</t>
   </si>
   <si>
@@ -49,6 +55,12 @@
     <t xml:space="preserve">file1.bin</t>
   </si>
   <si>
+    <t xml:space="preserve">2023-03-10 17:23:44</t>
+  </si>
+  <si>
+    <t xml:space="preserve">system</t>
+  </si>
+  <si>
     <t xml:space="preserve">TEST_3</t>
   </si>
   <si>
@@ -68,6 +80,12 @@
   </si>
   <si>
     <t xml:space="preserve">Notes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Modifier</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Modification Date</t>
   </si>
   <si>
     <t xml:space="preserve">&lt;b&gt;Test 1&lt;/b&gt;</t>
@@ -82,14 +100,21 @@
     <t xml:space="preserve">This is&gt;
 multiline
 text.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">test</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2023-03-11 17:23:44</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="General"/>
+    <numFmt numFmtId="165" formatCode="yyyy\-mm\-dd\ hh:mm:ss"/>
   </numFmts>
   <fonts count="7">
     <font>
@@ -180,7 +205,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -206,6 +231,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -234,10 +263,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AMJ15"/>
+  <dimension ref="A1:AMJ12"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B11" activeCellId="0" sqref="B11:B12"/>
+      <selection pane="topLeft" activeCell="A6" activeCellId="0" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.5234375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -247,6 +276,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="14.63"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="19"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="16.84"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="18.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="55"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1024" style="1" width="8.36"/>
   </cols>
@@ -278,27 +308,45 @@
       <c r="C4" s="5" t="s">
         <v>5</v>
       </c>
+      <c r="D4" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="5" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="6" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>8</v>
+        <v>10</v>
+      </c>
+      <c r="D5" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="6" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="C6" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D6" s="7" t="s">
         <v>11</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -315,48 +363,50 @@
     </row>
     <row r="10" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="B10" s="4"/>
     </row>
-    <row r="11" s="7" customFormat="true" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" s="8" customFormat="true" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="5" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="C11" s="5" t="s">
         <v>3</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>15</v>
+        <v>19</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>21</v>
       </c>
       <c r="AMJ11" s="1"/>
     </row>
     <row r="12" customFormat="false" ht="44" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="7" t="s">
-        <v>16</v>
+      <c r="A12" s="8" t="s">
+        <v>22</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="D12" s="8" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C13" s="0"/>
-    </row>
-    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B14" s="0"/>
-      <c r="C14" s="0"/>
-    </row>
-    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B15" s="0"/>
+        <v>24</v>
+      </c>
+      <c r="D12" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="F12" s="7" t="s">
+        <v>27</v>
+      </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>